<commit_message>
write some new for stephen
</commit_message>
<xml_diff>
--- a/character_expressions.xlsx
+++ b/character_expressions.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5377DD-ADBC-4B92-BDD2-4C3632925101}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C12B44-1104-4948-8100-0D0FC112C4A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70D50892-A28E-4BD4-8904-2E9A0AE59BDF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="436">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="662" uniqueCount="435">
   <si>
     <t>Mara</t>
   </si>
@@ -1035,9 +1035,6 @@
     <t>neutral indignant</t>
   </si>
   <si>
-    <t>neutral raised eyebrow</t>
-  </si>
-  <si>
     <t>neutral stern</t>
   </si>
   <si>
@@ -1218,9 +1215,6 @@
     <t>Petrov</t>
   </si>
   <si>
-    <t>neutral neutral_tears</t>
-  </si>
-  <si>
     <t>neutral crying_holding_back</t>
   </si>
   <si>
@@ -1342,6 +1336,9 @@
   </si>
   <si>
     <t>drinking_coffee satisfied</t>
+  </si>
+  <si>
+    <t>neutral tears</t>
   </si>
 </sst>
 </file>
@@ -1704,8 +1701,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3789E7F3-B1EE-45C8-97AD-43F0D15E3EB2}">
   <dimension ref="A1:L140"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B96" sqref="B96"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1740,25 +1737,25 @@
         <v>326</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
@@ -1778,7 +1775,7 @@
         <v>102</v>
       </c>
       <c r="F2" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -1828,7 +1825,7 @@
         <v>4</v>
       </c>
       <c r="J3" t="s">
-        <v>394</v>
+        <v>434</v>
       </c>
       <c r="K3" t="s">
         <v>29</v>
@@ -1866,13 +1863,13 @@
         <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="K4" t="s">
         <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
@@ -1892,10 +1889,10 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="G5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H5" t="s">
         <v>27</v>
@@ -1904,7 +1901,7 @@
         <v>101</v>
       </c>
       <c r="J5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="K5" t="s">
         <v>106</v>
@@ -1942,7 +1939,7 @@
         <v>27</v>
       </c>
       <c r="J6" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K6" t="s">
         <v>13</v>
@@ -1956,7 +1953,7 @@
         <v>105</v>
       </c>
       <c r="C7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -1968,7 +1965,7 @@
         <v>4</v>
       </c>
       <c r="G7" t="s">
-        <v>333</v>
+        <v>355</v>
       </c>
       <c r="H7" t="s">
         <v>28</v>
@@ -1977,10 +1974,10 @@
         <v>40</v>
       </c>
       <c r="J7" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="K7" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.3">
@@ -2038,7 +2035,7 @@
         <v>304</v>
       </c>
       <c r="H9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="I9" t="s">
         <v>18</v>
@@ -2105,7 +2102,7 @@
         <v>301</v>
       </c>
       <c r="I11" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="K11" t="s">
         <v>3</v>
@@ -2128,7 +2125,7 @@
         <v>9</v>
       </c>
       <c r="F12" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="G12" t="s">
         <v>43</v>
@@ -2140,7 +2137,7 @@
         <v>45</v>
       </c>
       <c r="K12" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -2163,7 +2160,7 @@
         <v>19</v>
       </c>
       <c r="G13" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="H13" t="s">
         <v>13</v>
@@ -2172,7 +2169,7 @@
         <v>25</v>
       </c>
       <c r="K13" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -2195,7 +2192,7 @@
         <v>303</v>
       </c>
       <c r="G14" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H14" t="s">
         <v>102</v>
@@ -2204,7 +2201,7 @@
         <v>301</v>
       </c>
       <c r="K14" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
@@ -2236,7 +2233,7 @@
         <v>15</v>
       </c>
       <c r="K15" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
@@ -2267,6 +2264,9 @@
       <c r="I16" t="s">
         <v>33</v>
       </c>
+      <c r="K16" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
@@ -2291,7 +2291,7 @@
         <v>45</v>
       </c>
       <c r="H17" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I17" t="s">
         <v>304</v>
@@ -2369,13 +2369,13 @@
         <v>302</v>
       </c>
       <c r="E20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="F20" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="G20" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H20" t="s">
         <v>57</v>
@@ -2401,13 +2401,16 @@
         <v>301</v>
       </c>
       <c r="F21" t="s">
-        <v>362</v>
+        <v>361</v>
+      </c>
+      <c r="G21" t="s">
+        <v>35</v>
       </c>
       <c r="H21" t="s">
         <v>54</v>
       </c>
       <c r="I21" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.3">
@@ -2429,11 +2432,14 @@
       <c r="F22" t="s">
         <v>305</v>
       </c>
+      <c r="G22" t="s">
+        <v>16</v>
+      </c>
       <c r="H22" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="I22" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -2459,7 +2465,7 @@
         <v>312</v>
       </c>
       <c r="I23" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
@@ -2485,7 +2491,7 @@
         <v>126</v>
       </c>
       <c r="I24" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
@@ -2502,10 +2508,10 @@
         <v>26</v>
       </c>
       <c r="E25" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="F25" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="H25" t="s">
         <v>119</v>
@@ -2531,7 +2537,7 @@
         <v>26</v>
       </c>
       <c r="F26" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H26" t="s">
         <v>48</v>
@@ -2560,7 +2566,7 @@
         <v>43</v>
       </c>
       <c r="H27" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
@@ -2623,10 +2629,10 @@
         <v>28</v>
       </c>
       <c r="E30" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F30" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
@@ -2663,10 +2669,10 @@
         <v>29</v>
       </c>
       <c r="E32" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F32" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
@@ -2691,7 +2697,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B34" t="s">
         <v>47</v>
@@ -2723,7 +2729,7 @@
         <v>34</v>
       </c>
       <c r="E35" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F35" t="s">
         <v>56</v>
@@ -2746,7 +2752,7 @@
         <v>32</v>
       </c>
       <c r="F36" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
@@ -2766,7 +2772,7 @@
         <v>34</v>
       </c>
       <c r="F37" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
@@ -2783,10 +2789,10 @@
         <v>309</v>
       </c>
       <c r="E38" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="F38" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
@@ -2803,7 +2809,7 @@
         <v>310</v>
       </c>
       <c r="E39" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="F39" t="s">
         <v>57</v>
@@ -2823,10 +2829,10 @@
         <v>311</v>
       </c>
       <c r="E40" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F40" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.3">
@@ -2843,10 +2849,10 @@
         <v>125</v>
       </c>
       <c r="E41" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="F41" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
@@ -2863,7 +2869,7 @@
         <v>51</v>
       </c>
       <c r="E42" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="F42" t="s">
         <v>48</v>
@@ -2937,10 +2943,10 @@
         <v>128</v>
       </c>
       <c r="C46" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="D46" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="E46" t="s">
         <v>54</v>
@@ -2960,13 +2966,13 @@
         <v>214</v>
       </c>
       <c r="D47" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="E47" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="F47" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
@@ -2980,13 +2986,13 @@
         <v>215</v>
       </c>
       <c r="D48" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="E48" t="s">
         <v>126</v>
       </c>
       <c r="F48" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
@@ -3006,7 +3012,7 @@
         <v>51</v>
       </c>
       <c r="F49" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
@@ -3023,10 +3029,10 @@
         <v>314</v>
       </c>
       <c r="E50" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F50" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
@@ -3046,7 +3052,7 @@
         <v>48</v>
       </c>
       <c r="F51" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
@@ -3066,7 +3072,7 @@
         <v>321</v>
       </c>
       <c r="F52" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
@@ -3086,7 +3092,7 @@
         <v>47</v>
       </c>
       <c r="F53" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
@@ -3100,13 +3106,13 @@
         <v>221</v>
       </c>
       <c r="D54" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="E54" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="F54" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
@@ -3123,7 +3129,7 @@
         <v>93</v>
       </c>
       <c r="E55" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F55" t="s">
         <v>124</v>
@@ -3163,7 +3169,7 @@
         <v>317</v>
       </c>
       <c r="E57" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
@@ -3180,7 +3186,7 @@
         <v>92</v>
       </c>
       <c r="E58" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
@@ -3202,7 +3208,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="B60" t="s">
         <v>142</v>
@@ -3222,7 +3228,7 @@
         <v>56</v>
       </c>
       <c r="B61" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="C61" t="s">
         <v>228</v>
@@ -3290,7 +3296,7 @@
         <v>60</v>
       </c>
       <c r="B65" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C65" t="s">
         <v>49</v>
@@ -3307,7 +3313,7 @@
         <v>61</v>
       </c>
       <c r="B66" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="C66" t="s">
         <v>231</v>
@@ -3316,7 +3322,7 @@
         <v>48</v>
       </c>
       <c r="E66" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.3">
@@ -3324,7 +3330,7 @@
         <v>62</v>
       </c>
       <c r="B67" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="C67" t="s">
         <v>232</v>
@@ -3341,7 +3347,7 @@
         <v>63</v>
       </c>
       <c r="B68" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="C68" t="s">
         <v>233</v>
@@ -3384,7 +3390,7 @@
         <v>324</v>
       </c>
       <c r="E70" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.3">
@@ -3401,12 +3407,12 @@
         <v>293</v>
       </c>
       <c r="E71" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="B72" t="s">
         <v>148</v>
@@ -3415,7 +3421,7 @@
         <v>237</v>
       </c>
       <c r="E72" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.3">
@@ -3429,7 +3435,7 @@
         <v>67</v>
       </c>
       <c r="E73" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.3">
@@ -3443,7 +3449,7 @@
         <v>238</v>
       </c>
       <c r="E74" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.3">
@@ -3457,7 +3463,7 @@
         <v>68</v>
       </c>
       <c r="E75" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.3">
@@ -3468,7 +3474,7 @@
         <v>152</v>
       </c>
       <c r="C76" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="E76" t="s">
         <v>146</v>
@@ -3485,7 +3491,7 @@
         <v>74</v>
       </c>
       <c r="E77" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.3">
@@ -3527,7 +3533,7 @@
         <v>241</v>
       </c>
       <c r="E80" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -3637,7 +3643,7 @@
         <v>85</v>
       </c>
       <c r="B90" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="C90" t="s">
         <v>251</v>
@@ -3645,7 +3651,7 @@
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="B91" t="s">
         <v>165</v>
@@ -3656,7 +3662,7 @@
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="B92" t="s">
         <v>166</v>
@@ -3692,7 +3698,7 @@
         <v>88</v>
       </c>
       <c r="B95" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="C95" t="s">
         <v>256</v>
@@ -3708,7 +3714,7 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C97" t="s">
         <v>258</v>
@@ -3716,7 +3722,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C98" t="s">
         <v>259</v>
@@ -3807,7 +3813,7 @@
         <v>97</v>
       </c>
       <c r="C109" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
@@ -3836,7 +3842,7 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C113" t="s">
         <v>273</v>
@@ -3844,7 +3850,7 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C114" t="s">
         <v>274</v>
@@ -3947,37 +3953,37 @@
     </row>
     <row r="134" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C134" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
     </row>
     <row r="135" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C135" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
     </row>
     <row r="136" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C136" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
     </row>
     <row r="137" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C137" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
     </row>
     <row r="138" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C138" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
     </row>
     <row r="139" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C139" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
     </row>
     <row r="140" spans="3:3" x14ac:dyDescent="0.3">
       <c r="C140" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
clean up some scripts
</commit_message>
<xml_diff>
--- a/character_expressions.xlsx
+++ b/character_expressions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\steph\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5718B9D-DFF6-4A63-A29E-70AFC2B9F2D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01409E13-7B1E-4F7C-B93C-5B66FBC77612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{70D50892-A28E-4BD4-8904-2E9A0AE59BDF}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="462">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="461">
   <si>
     <t>Mara</t>
   </si>
@@ -1389,21 +1389,6 @@
     <t>neutral indifferent</t>
   </si>
   <si>
-    <t>waving skeptical</t>
-  </si>
-  <si>
-    <t>waving annoyed</t>
-  </si>
-  <si>
-    <t>waving frustrated</t>
-  </si>
-  <si>
-    <t>waving away</t>
-  </si>
-  <si>
-    <t>waving cold</t>
-  </si>
-  <si>
     <t>Roxy</t>
   </si>
   <si>
@@ -1420,6 +1405,18 @@
   </si>
   <si>
     <t>eating smiling_nervous</t>
+  </si>
+  <si>
+    <t>arms_crossed cold</t>
+  </si>
+  <si>
+    <t>arms_crossed away</t>
+  </si>
+  <si>
+    <t>arms_crossed frustrated</t>
+  </si>
+  <si>
+    <t>neutral smiling_hostile</t>
   </si>
 </sst>
 </file>
@@ -1782,8 +1779,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3789E7F3-B1EE-45C8-97AD-43F0D15E3EB2}">
   <dimension ref="A1:N142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1835,7 +1832,7 @@
         <v>441</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>392</v>
@@ -2175,7 +2172,7 @@
         <v>449</v>
       </c>
       <c r="K9" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="M9" t="s">
         <v>26</v>
@@ -2438,7 +2435,7 @@
         <v>33</v>
       </c>
       <c r="J16" t="s">
-        <v>451</v>
+        <v>312</v>
       </c>
       <c r="K16" t="s">
         <v>416</v>
@@ -2476,7 +2473,7 @@
         <v>304</v>
       </c>
       <c r="J17" t="s">
-        <v>452</v>
+        <v>119</v>
       </c>
       <c r="K17" t="s">
         <v>39</v>
@@ -2511,7 +2508,7 @@
         <v>305</v>
       </c>
       <c r="J18" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="K18" t="s">
         <v>48</v>
@@ -2546,7 +2543,7 @@
         <v>57</v>
       </c>
       <c r="J19" t="s">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="K19" t="s">
         <v>49</v>
@@ -2581,7 +2578,7 @@
         <v>54</v>
       </c>
       <c r="J20" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
       <c r="K20" t="s">
         <v>230</v>
@@ -2616,10 +2613,10 @@
         <v>385</v>
       </c>
       <c r="J21" t="s">
-        <v>455</v>
+        <v>457</v>
       </c>
       <c r="K21" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
@@ -2653,6 +2650,9 @@
       <c r="J22" t="s">
         <v>442</v>
       </c>
+      <c r="K22" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
@@ -2879,6 +2879,9 @@
       <c r="H30" t="s">
         <v>49</v>
       </c>
+      <c r="J30" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
@@ -2899,6 +2902,9 @@
       <c r="F31" t="s">
         <v>125</v>
       </c>
+      <c r="J31" t="s">
+        <v>460</v>
+      </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
@@ -3717,7 +3723,7 @@
         <v>68</v>
       </c>
       <c r="D75" t="s">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E75" t="s">
         <v>351</v>
@@ -3768,7 +3774,7 @@
         <v>239</v>
       </c>
       <c r="D78" t="s">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="E78" t="s">
         <v>25</v>
@@ -3785,7 +3791,7 @@
         <v>240</v>
       </c>
       <c r="D79" t="s">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="E79" t="s">
         <v>45</v>

</xml_diff>